<commit_message>
REF-1089 To add instructions to Import file
REF-1089 To add instructions to Import file
</commit_message>
<xml_diff>
--- a/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
+++ b/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
@@ -1,31 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alekseymoseev/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{258C86A6-9716-8B40-B615-7AE31C2689D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A661ADA4-2367-314E-BAD9-E2C8E4A275CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6460" yWindow="2580" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24720" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PARTICIPANTS_TEMPLATE" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>First Name</t>
   </si>
@@ -60,29 +55,53 @@
     <t>Phone Type2</t>
   </si>
   <si>
-    <t>Street Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
     <t>Postal Code</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
     <t>Language</t>
+  </si>
+  <si>
+    <t>youremail@domain.com</t>
+  </si>
+  <si>
+    <t>Format per country</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Text ex. North Carolina</t>
+  </si>
+  <si>
+    <t>Enter either: Female
+Male</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD (formatted as text)
+ex. 2020-08-01</t>
+  </si>
+  <si>
+    <t>Format per country 
+919-555-1212</t>
+  </si>
+  <si>
+    <t>Enter either:
+Home
+Work
+Mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include language code if different from PI language </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -235,8 +254,17 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -414,20 +442,26 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="10">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4"/>
@@ -435,8 +469,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
@@ -444,8 +478,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.39997558519241921"/>
@@ -453,12 +487,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF7F7F7F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
@@ -468,12 +502,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -483,8 +517,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -492,12 +526,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="double">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="double">
+      </left>
+      <right style="double">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -507,12 +541,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FFB2B2B2"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
@@ -522,8 +556,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -533,7 +567,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -576,11 +610,18 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -614,6 +655,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -638,7 +680,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -791,25 +833,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110%"/>
-                <a:satMod val="105%"/>
-                <a:tint val="67%"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="103%"/>
-                <a:tint val="73%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="109%"/>
-                <a:tint val="81%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -817,25 +859,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103%"/>
-                <a:lumMod val="102%"/>
-                <a:tint val="94%"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110%"/>
-                <a:lumMod val="100%"/>
-                <a:shade val="100%"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99%"/>
-                <a:satMod val="120%"/>
-                <a:shade val="78%"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -848,21 +890,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -876,7 +918,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63%"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -888,32 +930,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95%"/>
-            <a:satMod val="170%"/>
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93%"/>
-                <a:satMod val="150%"/>
-                <a:shade val="98%"/>
-                <a:lumMod val="102%"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="98%"/>
-                <a:satMod val="130%"/>
-                <a:shade val="90%"/>
-                <a:lumMod val="103%"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63%"/>
-                <a:satMod val="120%"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -933,16 +975,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -982,20 +1036,335 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+    </row>
+    <row r="2" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="H2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
-        <v>16</v>
+      <c r="N2" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{54429226-1136-44D2-BA3D-64E90ADD09A7}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010044980BC293299A468BDFF2DF7D606875" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea17effd9695f7ed6f70ac8dd86d5b4">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b486ee1e-6752-4ccd-8230-71f87da8d43b" xmlns:ns4="50e20b6e-1115-4349-9356-b466c8d10314" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7452c8ae7df5a872c2f693b760efee7b" ns3:_="" ns4:_="">
+    <xsd:import namespace="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
+    <xsd:import namespace="50e20b6e-1115-4349-9356-b466c8d10314"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b486ee1e-6752-4ccd-8230-71f87da8d43b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="17" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="18" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="50e20b6e-1115-4349-9356-b466c8d10314" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="14" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058FB7F7-09D0-438D-8FE1-B8C0ED513C96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="50e20b6e-1115-4349-9356-b466c8d10314"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED183939-9121-41BC-B8E4-6FC63570EBFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
+    <ds:schemaRef ds:uri="50e20b6e-1115-4349-9356-b466c8d10314"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7632F0A1-E3D5-4EAD-A91F-760ED1F83686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
REF-189 import template fix
REF-189 import template fix
</commit_message>
<xml_diff>
--- a/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
+++ b/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alekseymoseev/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6642B7C-71AE-5A44-811A-AE8330049A24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7706EA-20D6-354B-A7DB-853959A03C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33360" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>First Name</t>
   </si>
@@ -79,25 +79,25 @@
     <t>Text capitalized as you want the name to appear in the platform.</t>
   </si>
   <si>
-    <t>May write out name or use intial with a period. Examples: 
-Mary or M.</t>
-  </si>
-  <si>
     <t>Enter spelled out as either: Female Male</t>
   </si>
   <si>
     <t>youremail@yourdomain.com</t>
   </si>
   <si>
-    <t>Enter one of these values: Home
-Work
-Mobile</t>
-  </si>
-  <si>
-    <t>State is required if applicable in your country. Spell out the state name. Example:   North Carolina</t>
-  </si>
-  <si>
     <t xml:space="preserve">Include ISO-2 language code if different from PI language.  </t>
+  </si>
+  <si>
+    <t>May write out name or use intial with a period. Examples:    Mary or M.</t>
+  </si>
+  <si>
+    <t>Enter one of these values: Home   Work  Mobile</t>
+  </si>
+  <si>
+    <t>Enter one of these values: Home        Work      Mobile</t>
+  </si>
+  <si>
+    <t>State is required if applicable in your country. Spell out the state name. Example: North Carolina</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1079,7 +1079,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>12</v>
@@ -1088,39 +1088,39 @@
         <v>12</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>11</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{9EFE8E52-DBC9-FD47-9B51-88CE0644F7AB}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{33EFD6C2-2161-0A46-80CE-ADCBE3F4F470}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>

</xml_diff>

<commit_message>
REF-2473 Bulk import Improvement and delegate functionality implemented
</commit_message>
<xml_diff>
--- a/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
+++ b/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alekseymoseev/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q1056549\Desktop\Participant_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7706EA-20D6-354B-A7DB-853959A03C38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{213A1BE9-D7DF-4579-AC05-D297EA7FA25A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33360" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PARTICIPANTS_TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>First Name</t>
   </si>
@@ -98,6 +98,21 @@
   </si>
   <si>
     <t>State is required if applicable in your country. Spell out the state name. Example: North Carolina</t>
+  </si>
+  <si>
+    <t>Delegate First Name</t>
+  </si>
+  <si>
+    <t>Delegate Last Name</t>
+  </si>
+  <si>
+    <t>Delegate Email</t>
+  </si>
+  <si>
+    <t>Delegate Phone Number</t>
+  </si>
+  <si>
+    <t>Delegate Phone Type</t>
   </si>
 </sst>
 </file>
@@ -1006,31 +1021,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" style="1"/>
-    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
     <col min="4" max="5" width="11" style="1"/>
-    <col min="6" max="6" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1"/>
-    <col min="10" max="10" width="17.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="11" style="1"/>
+    <col min="10" max="10" width="17.19921875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.296875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.19921875" style="1" customWidth="1"/>
+    <col min="15" max="17" width="11" style="1"/>
+    <col min="18" max="18" width="11" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1073,8 +1090,23 @@
       <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -1116,18 +1148,40 @@
       </c>
       <c r="N2" s="6" t="s">
         <v>21</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{33EFD6C2-2161-0A46-80CE-ADCBE3F4F470}"/>
+    <hyperlink ref="Q2" r:id="rId2" xr:uid="{235EFB7F-8DA8-4297-9E2F-A9614A9670C4}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010044980BC293299A468BDFF2DF7D606875" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea17effd9695f7ed6f70ac8dd86d5b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b486ee1e-6752-4ccd-8230-71f87da8d43b" xmlns:ns4="50e20b6e-1115-4349-9356-b466c8d10314" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7452c8ae7df5a872c2f693b760efee7b" ns3:_="" ns4:_="">
     <xsd:import namespace="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
@@ -1344,12 +1398,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1360,6 +1408,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058FB7F7-09D0-438D-8FE1-B8C0ED513C96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="50e20b6e-1115-4349-9356-b466c8d10314"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED183939-9121-41BC-B8E4-6FC63570EBFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1378,23 +1443,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058FB7F7-09D0-438D-8FE1-B8C0ED513C96}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="50e20b6e-1115-4349-9356-b466c8d10314"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7632F0A1-E3D5-4EAD-A91F-760ED1F83686}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Provided Jira details - REF-3292,REF-2927,REF-3242,REF-2473,REF-3282,REF-3285 - fix
</commit_message>
<xml_diff>
--- a/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
+++ b/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q1057161\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q1057161\Documents\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79FB29D8-85F2-4CE5-93CD-67E8B44FA491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351DFB52-0AFD-41E7-A4FE-BC2FD6BE213A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,31 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Middle Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Nickname</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Date of Birth</t>
-  </si>
-  <si>
-    <t>Email Address</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Phone Type</t>
   </si>
@@ -67,9 +43,6 @@
     <t>Format per country 919-555-1212</t>
   </si>
   <si>
-    <t>Alternative Phone</t>
-  </si>
-  <si>
     <t>Alt. Phone Type</t>
   </si>
   <si>
@@ -82,9 +55,6 @@
     <t>Enter spelled out as either: Female Male</t>
   </si>
   <si>
-    <t>youremail@yourdomain.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Include ISO-2 language code if different from PI language.  </t>
   </si>
   <si>
@@ -100,15 +70,50 @@
     <t>State is required if applicable in your country. Spell out the state name. Example: North Carolina</t>
   </si>
   <si>
-    <t>Delegate Phone Number</t>
-  </si>
-  <si>
-    <t>Delegate Phone Type</t>
+    <t>Primary Delegate First Name</t>
+  </si>
+  <si>
+    <t>Primary Delegate Last Name</t>
+  </si>
+  <si>
+    <t>Primary Delegate Email</t>
+  </si>
+  <si>
+    <t>Participant First Name</t>
+  </si>
+  <si>
+    <t>Participant Middle Name</t>
+  </si>
+  <si>
+    <t>Participant Last Name</t>
+  </si>
+  <si>
+    <t>Participant Nickname</t>
+  </si>
+  <si>
+    <t>Participant Sex</t>
+  </si>
+  <si>
+    <t>Participant Date of Birth</t>
+  </si>
+  <si>
+    <t>Participant Email Address</t>
+  </si>
+  <si>
+    <t>Participant Phone</t>
+  </si>
+  <si>
+    <t>Participant Alternative Phone</t>
+  </si>
+  <si>
+    <t>youremail@yourdomain.com If Participant is a minor the email address will not be stored</t>
+  </si>
+  <si>
+    <t>Format per country 919-555-1212.</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Text.
-</t>
+      <t xml:space="preserve">Format per country 919-555-1212       </t>
     </r>
     <r>
       <rPr>
@@ -119,12 +124,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Mandatory for Minor Participant</t>
+      <t>For a minor participant enter the participant delegate's phone number</t>
     </r>
   </si>
   <si>
     <r>
-      <t>Text.</t>
+      <t xml:space="preserve">Text.         </t>
     </r>
     <r>
       <rPr>
@@ -135,29 +140,40 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-Mandatory for Minor Participant</t>
+      <t>Mandatory for a minor participant</t>
     </r>
   </si>
   <si>
-    <t>Primary Delegate First Name</t>
-  </si>
-  <si>
-    <t>Primary Delegate Last Name</t>
-  </si>
-  <si>
-    <t>Primary Delegate Email</t>
-  </si>
-  <si>
-    <t>youremail@yourdomain.com 
-Mandatory for Minor Participant</t>
+    <r>
+      <t xml:space="preserve">Text.          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mandatory for a minor participant</t>
+    </r>
+  </si>
+  <si>
+    <t>youremail@yourdomain.com   Mandatory for a minor participant</t>
+  </si>
+  <si>
+    <t>Primary Delegate Phone Number</t>
+  </si>
+  <si>
+    <t>Primary Delegate Phone Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,13 +346,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -696,21 +705,25 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1071,18 +1084,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11" style="1"/>
+    <col min="1" max="1" width="13.08203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
     <col min="4" max="5" width="11" style="1"/>
     <col min="6" max="6" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1"/>
     <col min="10" max="10" width="17.1640625" style="1" customWidth="1"/>
@@ -1090,135 +1103,136 @@
     <col min="12" max="12" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.1640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.08203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.75" style="1" customWidth="1"/>
-    <col min="18" max="18" width="21.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="11" style="1"/>
+    <col min="15" max="15" width="17.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.25" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.9140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:19" s="6" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="J1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="O1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="6" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="N2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="108.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="Q2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{33EFD6C2-2161-0A46-80CE-ADCBE3F4F470}"/>
-    <hyperlink ref="Q2" r:id="rId2" xr:uid="{CD2056E9-C3C4-47FD-B10B-018BBE362AC2}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{D42CDB86-BC1C-450A-9846-0C4B9BD6223D}"/>
+    <hyperlink ref="Q2" r:id="rId2" xr:uid="{796D0DE0-D8C7-405E-BE22-3D6F657F3D77}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
@@ -1226,12 +1240,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010044980BC293299A468BDFF2DF7D606875" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea17effd9695f7ed6f70ac8dd86d5b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b486ee1e-6752-4ccd-8230-71f87da8d43b" xmlns:ns4="50e20b6e-1115-4349-9356-b466c8d10314" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7452c8ae7df5a872c2f693b760efee7b" ns3:_="" ns4:_="">
     <xsd:import namespace="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
@@ -1448,7 +1456,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1457,24 +1465,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058FB7F7-09D0-438D-8FE1-B8C0ED513C96}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="50e20b6e-1115-4349-9356-b466c8d10314"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED183939-9121-41BC-B8E4-6FC63570EBFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1493,10 +1490,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7632F0A1-E3D5-4EAD-A91F-760ED1F83686}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058FB7F7-09D0-438D-8FE1-B8C0ED513C96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="50e20b6e-1115-4349-9356-b466c8d10314"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
REF-3248- Bulk import fixes
</commit_message>
<xml_diff>
--- a/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
+++ b/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Q1061541\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q1056549\Desktop\25Aprilpackage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663496DE-1802-4554-B811-F2F3666B324D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F7A88C7-1685-41AD-9228-A4564BE6451F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PARTICIPANTS_TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Phone Type</t>
   </si>
@@ -199,6 +199,22 @@
   </si>
   <si>
     <t>Capitalized as you want the name to appear in the platform.    Text</t>
+  </si>
+  <si>
+    <t>Primary Delegate is over the age of legal majority</t>
+  </si>
+  <si>
+    <t>Enter one of these values:         Yes     
+ No</t>
+  </si>
+  <si>
+    <t>Primary Delegate Year of Birth</t>
+  </si>
+  <si>
+    <t>YYYY (formatted as text)</t>
+  </si>
+  <si>
+    <t>Country</t>
   </si>
 </sst>
 </file>
@@ -1116,36 +1132,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.08203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
     <col min="4" max="5" width="11" style="1"/>
-    <col min="6" max="6" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1"/>
-    <col min="10" max="10" width="17.1640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.25" style="1" customWidth="1"/>
-    <col min="17" max="17" width="28.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.9140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.19921875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.296875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.19921875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.296875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.19921875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="28.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -1179,32 +1195,41 @@
       <c r="K1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>29</v>
       </c>
+      <c r="U1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" s="6" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" s="6" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
@@ -1238,29 +1263,36 @@
       <c r="K2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="3"/>
+      <c r="M2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>30</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1271,15 +1303,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010044980BC293299A468BDFF2DF7D606875" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea17effd9695f7ed6f70ac8dd86d5b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b486ee1e-6752-4ccd-8230-71f87da8d43b" xmlns:ns4="50e20b6e-1115-4349-9356-b466c8d10314" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7452c8ae7df5a872c2f693b760efee7b" ns3:_="" ns4:_="">
     <xsd:import namespace="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
@@ -1496,6 +1519,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1503,14 +1535,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7632F0A1-E3D5-4EAD-A91F-760ED1F83686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED183939-9121-41BC-B8E4-6FC63570EBFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1525,6 +1549,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7632F0A1-E3D5-4EAD-A91F-760ED1F83686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
REF-3781 and REF-3248 fixes bulk import
</commit_message>
<xml_diff>
--- a/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
+++ b/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q1056549\Desktop\25Aprilpackage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q1057161\Desktop\Bulk_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F7A88C7-1685-41AD-9228-A4564BE6451F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA120803-1B0A-47DB-B848-CF288661C3CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="9080" yWindow="3520" windowWidth="10800" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PARTICIPANTS_TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
-  <si>
-    <t>Phone Type</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Postal Code</t>
   </si>
@@ -41,9 +38,6 @@
   </si>
   <si>
     <t>Format per country 919-555-1212</t>
-  </si>
-  <si>
-    <t>Alt. Phone Type</t>
   </si>
   <si>
     <t xml:space="preserve">State </t>
@@ -201,20 +195,91 @@
     <t>Capitalized as you want the name to appear in the platform.    Text</t>
   </si>
   <si>
-    <t>Primary Delegate is over the age of legal majority</t>
-  </si>
-  <si>
-    <t>Enter one of these values:         Yes     
- No</t>
-  </si>
-  <si>
-    <t>Primary Delegate Year of Birth</t>
-  </si>
-  <si>
-    <t>YYYY (formatted as text)</t>
-  </si>
-  <si>
     <t>Country</t>
+  </si>
+  <si>
+    <t>Participant Phone Type</t>
+  </si>
+  <si>
+    <t>Participant Alt. Phone Type</t>
+  </si>
+  <si>
+    <t>Primary Delegate YOB</t>
+  </si>
+  <si>
+    <t>YYYY (formatted as text) ex. 1987</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Mandatory for a minor participant. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Enter </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Yes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>attest the delegate is of/over the age of legal majority</t>
+    </r>
+  </si>
+  <si>
+    <t>Enter one of these values: Home         Work        Mobile</t>
+  </si>
+  <si>
+    <t>Confirm Primary Delegate is an adult</t>
   </si>
 </sst>
 </file>
@@ -750,7 +815,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -775,6 +840,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1134,165 +1202,169 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.09765625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.19921875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.08203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
     <col min="4" max="5" width="11" style="1"/>
-    <col min="6" max="6" width="28.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1"/>
-    <col min="10" max="10" width="17.19921875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.296875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.19921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.19921875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.296875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.19921875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="28.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11" style="1"/>
+    <col min="10" max="10" width="17.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="22.9140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.9140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="11" style="1"/>
+    <col min="22" max="22" width="17" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="6" customFormat="1" ht="78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="6" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="K1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" s="6" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" s="5" t="s">
+      <c r="T2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" s="6" customFormat="1" ht="124.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1303,6 +1375,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010044980BC293299A468BDFF2DF7D606875" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea17effd9695f7ed6f70ac8dd86d5b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b486ee1e-6752-4ccd-8230-71f87da8d43b" xmlns:ns4="50e20b6e-1115-4349-9356-b466c8d10314" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7452c8ae7df5a872c2f693b760efee7b" ns3:_="" ns4:_="">
     <xsd:import namespace="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
@@ -1519,15 +1600,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1535,6 +1607,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7632F0A1-E3D5-4EAD-A91F-760ED1F83686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED183939-9121-41BC-B8E4-6FC63570EBFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1549,14 +1629,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7632F0A1-E3D5-4EAD-A91F-760ED1F83686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Jira-REF-4016 and REF-4034 and REF-2490
</commit_message>
<xml_diff>
--- a/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
+++ b/force-app/main/default/staticresources/PARTICIPANTS_TEMPLATE.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q1058838\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q1057161\Desktop\Bulk_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9120BD8-B78D-4FD3-ADD8-C39D66A03392}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5CE6C4-FC5E-4F06-893E-2A7568437B03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Enter spelled out as either: Female Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include ISO-2 language code if different from PI language.  </t>
   </si>
   <si>
     <t>May write out name or use intial with a period. Examples:    Mary or M.</t>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>AM/PM</t>
+  </si>
+  <si>
+    <t>Include ISO-2 language code if different from PI language or leave blank if ISO-2 code is unknown</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1228,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1258,40 +1258,40 @@
   <sheetData>
     <row r="1" spans="1:25" s="6" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="L1" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>6</v>
@@ -1300,45 +1300,45 @@
         <v>0</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="S1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="V1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="X1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="6" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>3</v>
@@ -1353,61 +1353,61 @@
         <v>4</v>
       </c>
       <c r="G2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="S2" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +1429,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1438,21 +1438,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010044980BC293299A468BDFF2DF7D606875" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0ea17effd9695f7ed6f70ac8dd86d5b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b486ee1e-6752-4ccd-8230-71f87da8d43b" xmlns:ns4="50e20b6e-1115-4349-9356-b466c8d10314" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7452c8ae7df5a872c2f693b760efee7b" ns3:_="" ns4:_="">
     <xsd:import namespace="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
@@ -1669,32 +1654,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7632F0A1-E3D5-4EAD-A91F-760ED1F83686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058FB7F7-09D0-438D-8FE1-B8C0ED513C96}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="50e20b6e-1115-4349-9356-b466c8d10314"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED183939-9121-41BC-B8E4-6FC63570EBFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1711,4 +1686,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7632F0A1-E3D5-4EAD-A91F-760ED1F83686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058FB7F7-09D0-438D-8FE1-B8C0ED513C96}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b486ee1e-6752-4ccd-8230-71f87da8d43b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="50e20b6e-1115-4349-9356-b466c8d10314"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>